<commit_message>
feat: fix bash script input data and project configs
</commit_message>
<xml_diff>
--- a/src/L5zero/localization.xlsx
+++ b/src/L5zero/localization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rumyantsev\IdeaProjects\bookshop\src\L5zero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rumyantsev\IdeaProjects\bookshop\front\bookshop-front\src\L5zero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A27ECD-6090-4E9E-8318-78B30246DE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F0553-80B1-4A65-97FD-61EDE931B706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3690" windowWidth="17370" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="166">
   <si>
     <t>key</t>
   </si>
@@ -39,184 +39,490 @@
     <t>ru</t>
   </si>
   <si>
-    <t>user registered successfully</t>
-  </si>
-  <si>
-    <t>Пользователь успешно зарегистрирован</t>
-  </si>
-  <si>
-    <t>user_exists</t>
-  </si>
-  <si>
-    <t>user already exists</t>
-  </si>
-  <si>
-    <t>Пользователь уже существует</t>
-  </si>
-  <si>
-    <t>file_empty</t>
-  </si>
-  <si>
-    <t>file is empty!</t>
-  </si>
-  <si>
-    <t>Файл пуст!</t>
-  </si>
-  <si>
-    <t>extractor not found</t>
-  </si>
-  <si>
-    <t>extractor_not_found</t>
-  </si>
-  <si>
-    <t>Экстратор не найден</t>
-  </si>
-  <si>
-    <t>no_access</t>
-  </si>
-  <si>
-    <t>Нет доступа!</t>
-  </si>
-  <si>
-    <t>no access!</t>
-  </si>
-  <si>
-    <t>user_not_found</t>
-  </si>
-  <si>
-    <t>user not found</t>
-  </si>
-  <si>
-    <t>Пользователь не найден</t>
-  </si>
-  <si>
-    <t>wrong_extension</t>
-  </si>
-  <si>
-    <t>wrong extension!</t>
-  </si>
-  <si>
-    <t>Неверное расширение</t>
-  </si>
-  <si>
-    <t>error_reading_bytes</t>
-  </si>
-  <si>
-    <t>error reading bytes</t>
-  </si>
-  <si>
-    <t>could_not_extract</t>
-  </si>
-  <si>
-    <t>could not extract content</t>
-  </si>
-  <si>
-    <t>Ошибка при чтении байтов</t>
-  </si>
-  <si>
-    <t>Невозможно извлечь содержимое</t>
-  </si>
-  <si>
-    <t>error_loading_doc</t>
-  </si>
-  <si>
-    <t>error loading document</t>
-  </si>
-  <si>
-    <t>Ошибка при загрузке документа</t>
-  </si>
-  <si>
-    <t>error_closing_doc</t>
-  </si>
-  <si>
-    <t>error closing document</t>
-  </si>
-  <si>
-    <t>Ошибка при закрытии документа</t>
-  </si>
-  <si>
-    <t>error_cover_image</t>
-  </si>
-  <si>
-    <t>error while creating cover image</t>
-  </si>
-  <si>
-    <t>Ошибка при создании обложки</t>
-  </si>
-  <si>
-    <t>error_writing_img</t>
-  </si>
-  <si>
-    <t>error while writing image to stream</t>
-  </si>
-  <si>
-    <t>Ошибка при записи картинки в поток</t>
-  </si>
-  <si>
-    <t>file_not_found</t>
-  </si>
-  <si>
-    <t>book_not_found</t>
-  </si>
-  <si>
-    <t>file not found</t>
-  </si>
-  <si>
-    <t>book not found</t>
-  </si>
-  <si>
-    <t>Файл не найден</t>
-  </si>
-  <si>
-    <t>Книга не найдена</t>
-  </si>
-  <si>
-    <t>comment_not_found</t>
-  </si>
-  <si>
-    <t>cooment not found</t>
-  </si>
-  <si>
-    <t>Комментарий не найден</t>
-  </si>
-  <si>
-    <t>file_write_error</t>
-  </si>
-  <si>
-    <t>error writing file</t>
-  </si>
-  <si>
-    <t>Ошибка при записи в файл</t>
-  </si>
-  <si>
-    <t>file_read_error</t>
-  </si>
-  <si>
-    <t>error while reading file</t>
-  </si>
-  <si>
-    <t>Ошибка чтения файла</t>
-  </si>
-  <si>
-    <t>file_no_name_error</t>
-  </si>
-  <si>
-    <t>files without name are not supperted</t>
-  </si>
-  <si>
-    <t>Файлы без имени не поддерживаются</t>
-  </si>
-  <si>
-    <t>error_removing_file</t>
-  </si>
-  <si>
-    <t>error removing a file</t>
-  </si>
-  <si>
-    <t>Ошибка при удалении файла</t>
-  </si>
-  <si>
-    <t>success_registration</t>
+    <t>download</t>
+  </si>
+  <si>
+    <t>download button text</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>card desc title</t>
+  </si>
+  <si>
+    <t>card desc author</t>
+  </si>
+  <si>
+    <t>card desc genre</t>
+  </si>
+  <si>
+    <t>DOWNLOAD</t>
+  </si>
+  <si>
+    <t>СКАЧАТЬ</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Автор</t>
+  </si>
+  <si>
+    <t>Жанр</t>
+  </si>
+  <si>
+    <t>addComment</t>
+  </si>
+  <si>
+    <t>add comment button</t>
+  </si>
+  <si>
+    <t>LEAVE A COMMENT</t>
+  </si>
+  <si>
+    <t>ОСТАВИТЬ КОММЕНТАРИЙ</t>
+  </si>
+  <si>
+    <t>emptyDescription</t>
+  </si>
+  <si>
+    <t>empty description</t>
+  </si>
+  <si>
+    <t>NO DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ОПИСАНИЯ НЕТ</t>
+  </si>
+  <si>
+    <t>editBook</t>
+  </si>
+  <si>
+    <t>edit Book header(modal)</t>
+  </si>
+  <si>
+    <t>Edit book</t>
+  </si>
+  <si>
+    <t>Редактировать книгу</t>
+  </si>
+  <si>
+    <t>book edit form label</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>modal button</t>
+  </si>
+  <si>
+    <t>SAVE</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>СОХРАНИТЬ</t>
+  </si>
+  <si>
+    <t>УДАЛИТЬ</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>catalog</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>header menu button</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>Log out</t>
+  </si>
+  <si>
+    <t>Профиль</t>
+  </si>
+  <si>
+    <t>Каталог</t>
+  </si>
+  <si>
+    <t>Выход</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>Войти</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>sortingOldest</t>
+  </si>
+  <si>
+    <t>sortingNewest</t>
+  </si>
+  <si>
+    <t>sortByAuthor</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+  <si>
+    <t>sorting option</t>
+  </si>
+  <si>
+    <t>Сначала старые</t>
+  </si>
+  <si>
+    <t>Oldest first</t>
+  </si>
+  <si>
+    <t>Newest first</t>
+  </si>
+  <si>
+    <t>Сначала новые</t>
+  </si>
+  <si>
+    <t>By title</t>
+  </si>
+  <si>
+    <t>By author</t>
+  </si>
+  <si>
+    <t>По названию</t>
+  </si>
+  <si>
+    <t>По автору</t>
+  </si>
+  <si>
+    <t>search bar label</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Поиск</t>
+  </si>
+  <si>
+    <t>next catalog button</t>
+  </si>
+  <si>
+    <t>prev catalog button</t>
+  </si>
+  <si>
+    <t>След.</t>
+  </si>
+  <si>
+    <t>Пред.</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>sortByTitle</t>
+  </si>
+  <si>
+    <t>uploadDialogTitle</t>
+  </si>
+  <si>
+    <t>dialog title</t>
+  </si>
+  <si>
+    <t>Upload a File</t>
+  </si>
+  <si>
+    <t>Загрузка файла</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>dialog button</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>UPLOAD</t>
+  </si>
+  <si>
+    <t>ОТМЕНА</t>
+  </si>
+  <si>
+    <t>ЗАГРУЗИТЬ</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>profile title</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>regDate</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Registration date</t>
+  </si>
+  <si>
+    <t>Имя пользователя</t>
+  </si>
+  <si>
+    <t>Почта</t>
+  </si>
+  <si>
+    <t>Дата регистрации</t>
+  </si>
+  <si>
+    <t>changeCreds</t>
+  </si>
+  <si>
+    <t>profile button</t>
+  </si>
+  <si>
+    <t>CHANGE CREDENTIALS</t>
+  </si>
+  <si>
+    <t>Изменить данные</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>profile form text</t>
+  </si>
+  <si>
+    <t>confirmPass</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>viewProfile</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm password</t>
+  </si>
+  <si>
+    <t>SUBMIT</t>
+  </si>
+  <si>
+    <t>VIEW PROFILE</t>
+  </si>
+  <si>
+    <t>Пароль</t>
+  </si>
+  <si>
+    <t>Подтверждение пароля</t>
+  </si>
+  <si>
+    <t>ОТПРАВИТЬ</t>
+  </si>
+  <si>
+    <t>ВЕРНУТЬСЯ В ПРОФИЛЬ</t>
+  </si>
+  <si>
+    <t>usernameError</t>
+  </si>
+  <si>
+    <t>regform error</t>
+  </si>
+  <si>
+    <t>passwordError</t>
+  </si>
+  <si>
+    <t>confirmPassError</t>
+  </si>
+  <si>
+    <t>emailError</t>
+  </si>
+  <si>
+    <t>Please enter only English alphabets and numbers</t>
+  </si>
+  <si>
+    <t>Symbols in password are not allowed</t>
+  </si>
+  <si>
+    <t>Passwords do not match</t>
+  </si>
+  <si>
+    <t>Invalid email address</t>
+  </si>
+  <si>
+    <t>Разрешены только буквы английского алфавита и цифры</t>
+  </si>
+  <si>
+    <t>Не используйте специальные символы в пароле</t>
+  </si>
+  <si>
+    <t>Пароли не совпадают</t>
+  </si>
+  <si>
+    <t>Неверный email</t>
+  </si>
+  <si>
+    <t>commentDialogTitle</t>
+  </si>
+  <si>
+    <t>Enter comment text</t>
+  </si>
+  <si>
+    <t>Введите комментарий</t>
+  </si>
+  <si>
+    <t>input label</t>
+  </si>
+  <si>
+    <t>commentFormLabel</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Комментарий</t>
+  </si>
+  <si>
+    <t>getBooksError</t>
+  </si>
+  <si>
+    <t>Error while getting books from server</t>
+  </si>
+  <si>
+    <t>Ошибка при получении книг:</t>
+  </si>
+  <si>
+    <t>Error while getting books:</t>
+  </si>
+  <si>
+    <t>editBookError</t>
+  </si>
+  <si>
+    <t>Validation error</t>
+  </si>
+  <si>
+    <t>Invalid input. Only English and Russian characters are allowed.</t>
+  </si>
+  <si>
+    <t>Разрешены только буквы английского и русского алфавитов</t>
+  </si>
+  <si>
+    <t>Ошибка при загрузке изображения:</t>
+  </si>
+  <si>
+    <t>getImageError</t>
+  </si>
+  <si>
+    <t>Error while getting image</t>
+  </si>
+  <si>
+    <t>Error while getting image:</t>
+  </si>
+  <si>
+    <t>loadingImage</t>
+  </si>
+  <si>
+    <t>Image loading message</t>
+  </si>
+  <si>
+    <t>Image loading...</t>
+  </si>
+  <si>
+    <t>Загрузка изображения...</t>
+  </si>
+  <si>
+    <t>getPreviewError</t>
+  </si>
+  <si>
+    <t>Error while getting preview</t>
+  </si>
+  <si>
+    <t>Error while getting preview:</t>
+  </si>
+  <si>
+    <t>Ошибка при получении превью:</t>
+  </si>
+  <si>
+    <t>uploadError</t>
+  </si>
+  <si>
+    <t>Error uploading file</t>
+  </si>
+  <si>
+    <t>Upload error:</t>
+  </si>
+  <si>
+    <t>Ошибка при загрузке:</t>
+  </si>
+  <si>
+    <t>getProfileDataError</t>
+  </si>
+  <si>
+    <t>Error getting profile data</t>
+  </si>
+  <si>
+    <t>Error while getting profile data:</t>
+  </si>
+  <si>
+    <t>Ошибка при получении данных профиля:</t>
   </si>
 </sst>
 </file>
@@ -583,13 +889,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,235 +919,634 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>79</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>60</v>
+      <c r="B21" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>